<commit_message>
example 4 with cpp
</commit_message>
<xml_diff>
--- a/examples/04_two_state_disability/base_assumption.xlsx
+++ b/examples/04_two_state_disability/base_assumption.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="22515" windowHeight="11070" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="22515" windowHeight="11070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MORTALITY (0-&gt;3)" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="DIS_DEATH2 (2-&gt;3)" sheetId="10" r:id="rId9"/>
     <sheet name="REC2(2-&gt;0)" sheetId="7" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -1799,7 +1799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1841,10 +1841,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B154"/>
+  <dimension ref="A1:B155"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B5" s="1">
         <v>0.05</v>
@@ -1883,407 +1883,407 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>2023</v>
-      </c>
-      <c r="B6" s="4">
-        <v>4.9000000000000002E-2</v>
+        <v>2022</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>2024</v>
-      </c>
-      <c r="B7" s="1">
-        <v>4.8000000000000001E-2</v>
+        <v>2023</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>2025</v>
-      </c>
-      <c r="B8" s="4">
-        <v>4.7E-2</v>
+        <v>2024</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>2026</v>
-      </c>
-      <c r="B9" s="1">
-        <v>4.5999999999999999E-2</v>
+        <v>2025</v>
+      </c>
+      <c r="B9" s="4">
+        <v>4.7E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>2027</v>
-      </c>
-      <c r="B10" s="4">
-        <v>4.4999999999999998E-2</v>
+        <v>2026</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>2028</v>
-      </c>
-      <c r="B11" s="1">
-        <v>4.3999999999999997E-2</v>
+        <v>2027</v>
+      </c>
+      <c r="B11" s="4">
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>2029</v>
-      </c>
-      <c r="B12" s="4">
-        <v>4.2999999999999997E-2</v>
+        <v>2028</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>2030</v>
-      </c>
-      <c r="B13" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>2029</v>
+      </c>
+      <c r="B13" s="4">
+        <v>4.2999999999999997E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>2031</v>
-      </c>
-      <c r="B14" s="4">
-        <v>4.1000000000000002E-2</v>
+        <v>2030</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>2032</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0.04</v>
+        <v>2031</v>
+      </c>
+      <c r="B15" s="4">
+        <v>4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>2033</v>
-      </c>
-      <c r="B16" s="4">
-        <v>3.9E-2</v>
+        <v>2032</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.04</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>2034</v>
-      </c>
-      <c r="B17" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>2033</v>
+      </c>
+      <c r="B17" s="4">
+        <v>3.9E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>2035</v>
-      </c>
-      <c r="B18" s="4">
-        <v>3.6999999999999998E-2</v>
+        <v>2034</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3.7999999999999999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>2036</v>
-      </c>
-      <c r="B19" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>2035</v>
+      </c>
+      <c r="B19" s="4">
+        <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>2037</v>
-      </c>
-      <c r="B20" s="4">
-        <v>3.5000000000000003E-2</v>
+        <v>2036</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>2038</v>
-      </c>
-      <c r="B21" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>2037</v>
+      </c>
+      <c r="B21" s="4">
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>2039</v>
-      </c>
-      <c r="B22" s="4">
-        <v>3.3000000000000002E-2</v>
+        <v>2038</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>2040</v>
-      </c>
-      <c r="B23" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>2039</v>
+      </c>
+      <c r="B23" s="4">
+        <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>2041</v>
-      </c>
-      <c r="B24" s="4">
-        <v>3.1E-2</v>
+        <v>2040</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>2042</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0.03</v>
+        <v>2041</v>
+      </c>
+      <c r="B25" s="4">
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>2043</v>
-      </c>
-      <c r="B26" s="4">
-        <v>2.9000000000000001E-2</v>
+        <v>2042</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.03</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>2044</v>
-      </c>
-      <c r="B27" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>2043</v>
+      </c>
+      <c r="B27" s="4">
+        <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>2045</v>
-      </c>
-      <c r="B28" s="4">
-        <v>2.7E-2</v>
+        <v>2044</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>2046</v>
-      </c>
-      <c r="B29" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>2045</v>
+      </c>
+      <c r="B29" s="4">
+        <v>2.7E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>2047</v>
-      </c>
-      <c r="B30" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>2046</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>2048</v>
-      </c>
-      <c r="B31" s="1">
-        <v>2.4E-2</v>
+        <v>2047</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>2049</v>
-      </c>
-      <c r="B32" s="4">
-        <v>2.3E-2</v>
+        <v>2048</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>2050</v>
-      </c>
-      <c r="B33" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>2049</v>
+      </c>
+      <c r="B33" s="4">
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>2051</v>
-      </c>
-      <c r="B34" s="4">
-        <v>2.1000000000000001E-2</v>
+        <v>2050</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>2052</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0.02</v>
+        <v>2051</v>
+      </c>
+      <c r="B35" s="4">
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>2053</v>
-      </c>
-      <c r="B36" s="4">
-        <v>1.9E-2</v>
+        <v>2052</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.02</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>2054</v>
-      </c>
-      <c r="B37" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>2053</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>2055</v>
-      </c>
-      <c r="B38" s="4">
-        <v>1.7000000000000001E-2</v>
+        <v>2054</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>2056</v>
-      </c>
-      <c r="B39" s="1">
-        <v>1.6E-2</v>
+        <v>2055</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>2057</v>
-      </c>
-      <c r="B40" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>2056</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>2058</v>
-      </c>
-      <c r="B41" s="1">
-        <v>1.4E-2</v>
+        <v>2057</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>2059</v>
-      </c>
-      <c r="B42" s="4">
-        <v>1.2999999999999999E-2</v>
+        <v>2058</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>2060</v>
-      </c>
-      <c r="B43" s="1">
-        <v>1.2E-2</v>
+        <v>2059</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>2061</v>
-      </c>
-      <c r="B44" s="4">
-        <v>1.0999999999999999E-2</v>
+        <v>2060</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>2062</v>
-      </c>
-      <c r="B45" s="1">
-        <v>0.01</v>
+        <v>2061</v>
+      </c>
+      <c r="B45" s="4">
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>2063</v>
-      </c>
-      <c r="B46" s="4">
-        <v>8.9999999999999993E-3</v>
+        <v>2062</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.01</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>2064</v>
-      </c>
-      <c r="B47" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>2063</v>
+      </c>
+      <c r="B47" s="4">
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>2065</v>
-      </c>
-      <c r="B48" s="4">
-        <v>7.0000000000000097E-3</v>
+        <v>2064</v>
+      </c>
+      <c r="B48" s="1">
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>2066</v>
-      </c>
-      <c r="B49" s="1">
-        <v>6.0000000000000097E-3</v>
+        <v>2065</v>
+      </c>
+      <c r="B49" s="4">
+        <v>7.0000000000000097E-3</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>2067</v>
-      </c>
-      <c r="B50" s="4">
-        <v>5.0000000000000001E-3</v>
+        <v>2066</v>
+      </c>
+      <c r="B50" s="1">
+        <v>6.0000000000000097E-3</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>2068</v>
-      </c>
-      <c r="B51" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>2067</v>
+      </c>
+      <c r="B51" s="4">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>2069</v>
-      </c>
-      <c r="B52" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>2068</v>
+      </c>
+      <c r="B52" s="1">
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>2070</v>
-      </c>
-      <c r="B53" s="1">
-        <v>2E-3</v>
+        <v>2069</v>
+      </c>
+      <c r="B53" s="4">
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <v>2071</v>
-      </c>
-      <c r="B54" s="4">
-        <v>1E-3</v>
+        <v>2070</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>2072</v>
-      </c>
-      <c r="B55" s="1">
-        <v>0</v>
+        <v>2071</v>
+      </c>
+      <c r="B55" s="4">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="B57" s="1">
         <v>0</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="B63" s="1">
         <v>0</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="B64" s="1">
         <v>0</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="B65" s="1">
         <v>0</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B67" s="1">
         <v>0</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="B68" s="1">
         <v>0</v>
@@ -2387,7 +2387,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="B69" s="1">
         <v>0</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="B71" s="1">
         <v>0</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="B73" s="1">
         <v>0</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="B74" s="1">
         <v>0</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="B75" s="1">
         <v>0</v>
@@ -2443,7 +2443,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="B76" s="1">
         <v>0</v>
@@ -2451,7 +2451,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="B77" s="1">
         <v>0</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="B78" s="1">
         <v>0</v>
@@ -2467,7 +2467,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B79" s="1">
         <v>0</v>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="B80" s="1">
         <v>0</v>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="B81" s="1">
         <v>0</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="B82" s="1">
         <v>0</v>
@@ -2499,7 +2499,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="B83" s="1">
         <v>0</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="B84" s="1">
         <v>0</v>
@@ -2515,7 +2515,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="B85" s="1">
         <v>0</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="B86" s="1">
         <v>0</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="B87" s="1">
         <v>0</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="B88" s="1">
         <v>0</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="B89" s="1">
         <v>0</v>
@@ -2555,7 +2555,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="B90" s="1">
         <v>0</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="B91" s="1">
         <v>0</v>
@@ -2571,7 +2571,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="B92" s="1">
         <v>0</v>
@@ -2579,7 +2579,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="B93" s="1">
         <v>0</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="B94" s="1">
         <v>0</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="B95" s="1">
         <v>0</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="B96" s="1">
         <v>0</v>
@@ -2611,7 +2611,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="B97" s="1">
         <v>0</v>
@@ -2619,7 +2619,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="B98" s="1">
         <v>0</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="B99" s="1">
         <v>0</v>
@@ -2635,7 +2635,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="B100" s="1">
         <v>0</v>
@@ -2643,7 +2643,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="B101" s="1">
         <v>0</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="B102" s="1">
         <v>0</v>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="B103" s="1">
         <v>0</v>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="B104" s="1">
         <v>0</v>
@@ -2675,7 +2675,7 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="B105" s="1">
         <v>0</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="106" spans="1:2">
       <c r="A106">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="B106" s="1">
         <v>0</v>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="B107" s="1">
         <v>0</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="B108" s="1">
         <v>0</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="109" spans="1:2">
       <c r="A109">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="B109" s="1">
         <v>0</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="B110" s="1">
         <v>0</v>
@@ -2723,7 +2723,7 @@
     </row>
     <row r="111" spans="1:2">
       <c r="A111">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="B111" s="1">
         <v>0</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="112" spans="1:2">
       <c r="A112">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="B112" s="1">
         <v>0</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="113" spans="1:2">
       <c r="A113">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="B113" s="1">
         <v>0</v>
@@ -2747,7 +2747,7 @@
     </row>
     <row r="114" spans="1:2">
       <c r="A114">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="B114" s="1">
         <v>0</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="115" spans="1:2">
       <c r="A115">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="B115" s="1">
         <v>0</v>
@@ -2763,7 +2763,7 @@
     </row>
     <row r="116" spans="1:2">
       <c r="A116">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="B116" s="1">
         <v>0</v>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="117" spans="1:2">
       <c r="A117">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="B117" s="1">
         <v>0</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="118" spans="1:2">
       <c r="A118">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="B118" s="1">
         <v>0</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="B119" s="1">
         <v>0</v>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="120" spans="1:2">
       <c r="A120">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="B120" s="1">
         <v>0</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="B121" s="1">
         <v>0</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="B122" s="1">
         <v>0</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="B123" s="1">
         <v>0</v>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="124" spans="1:2">
       <c r="A124">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="B124" s="1">
         <v>0</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="125" spans="1:2">
       <c r="A125">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="B125" s="1">
         <v>0</v>
@@ -2843,7 +2843,7 @@
     </row>
     <row r="126" spans="1:2">
       <c r="A126">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="B126" s="1">
         <v>0</v>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="127" spans="1:2">
       <c r="A127">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="B127" s="1">
         <v>0</v>
@@ -2859,7 +2859,7 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="B128" s="1">
         <v>0</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="129" spans="1:2">
       <c r="A129">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="B129" s="1">
         <v>0</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="130" spans="1:2">
       <c r="A130">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B130" s="1">
         <v>0</v>
@@ -2883,7 +2883,7 @@
     </row>
     <row r="131" spans="1:2">
       <c r="A131">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="B131" s="1">
         <v>0</v>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="132" spans="1:2">
       <c r="A132">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="B132" s="1">
         <v>0</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="133" spans="1:2">
       <c r="A133">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="B133" s="1">
         <v>0</v>
@@ -2907,7 +2907,7 @@
     </row>
     <row r="134" spans="1:2">
       <c r="A134">
-        <v>2151</v>
+        <v>2150</v>
       </c>
       <c r="B134" s="1">
         <v>0</v>
@@ -2915,7 +2915,7 @@
     </row>
     <row r="135" spans="1:2">
       <c r="A135">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="B135" s="1">
         <v>0</v>
@@ -2923,7 +2923,7 @@
     </row>
     <row r="136" spans="1:2">
       <c r="A136">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="B136" s="1">
         <v>0</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="137" spans="1:2">
       <c r="A137">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="B137" s="1">
         <v>0</v>
@@ -2939,7 +2939,7 @@
     </row>
     <row r="138" spans="1:2">
       <c r="A138">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="B138" s="1">
         <v>0</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="139" spans="1:2">
       <c r="A139">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="B139" s="1">
         <v>0</v>
@@ -2955,7 +2955,7 @@
     </row>
     <row r="140" spans="1:2">
       <c r="A140">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="B140" s="1">
         <v>0</v>
@@ -2963,7 +2963,7 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="B141" s="1">
         <v>0</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="142" spans="1:2">
       <c r="A142">
-        <v>2159</v>
+        <v>2158</v>
       </c>
       <c r="B142" s="1">
         <v>0</v>
@@ -2979,7 +2979,7 @@
     </row>
     <row r="143" spans="1:2">
       <c r="A143">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="B143" s="1">
         <v>0</v>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="B144" s="1">
         <v>0</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="145" spans="1:2">
       <c r="A145">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="B145" s="1">
         <v>0</v>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="146" spans="1:2">
       <c r="A146">
-        <v>2163</v>
+        <v>2162</v>
       </c>
       <c r="B146" s="1">
         <v>0</v>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="147" spans="1:2">
       <c r="A147">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="B147" s="1">
         <v>0</v>
@@ -3019,7 +3019,7 @@
     </row>
     <row r="148" spans="1:2">
       <c r="A148">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="B148" s="1">
         <v>0</v>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="149" spans="1:2">
       <c r="A149">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="B149" s="1">
         <v>0</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="150" spans="1:2">
       <c r="A150">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="B150" s="1">
         <v>0</v>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="151" spans="1:2">
       <c r="A151">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="B151" s="1">
         <v>0</v>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="152" spans="1:2">
       <c r="A152">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="B152" s="1">
         <v>0</v>
@@ -3059,7 +3059,7 @@
     </row>
     <row r="153" spans="1:2">
       <c r="A153">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="B153" s="1">
         <v>0</v>
@@ -3067,9 +3067,17 @@
     </row>
     <row r="154" spans="1:2">
       <c r="A154">
+        <v>2170</v>
+      </c>
+      <c r="B154" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155">
         <v>2171</v>
       </c>
-      <c r="B154" s="1">
+      <c r="B155" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4234,7 +4242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B124"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A125" sqref="A125:B157"/>
     </sheetView>
   </sheetViews>

</xml_diff>